<commit_message>
Added father_alive field to fixtures and importer
</commit_message>
<xml_diff>
--- a/spec/fixtures/one_orphan_xlsx.xlsx
+++ b/spec/fixtures/one_orphan_xlsx.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <workbookPr autoCompressPictures="0"/>
+  <bookViews>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" tabRatio="500"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>الرقم المسلسل</t>
   </si>
@@ -109,7 +117,7 @@
     <t>ملاحظات</t>
   </si>
   <si>
-    <t>الاسم </t>
+    <t>الاسم</t>
   </si>
   <si>
     <t>صلة القرابة</t>
@@ -124,7 +132,7 @@
     <t>المدينة</t>
   </si>
   <si>
-    <t>الحي </t>
+    <t>الحي</t>
   </si>
   <si>
     <t>الشارع</t>
@@ -139,7 +147,7 @@
     <t>المدينة</t>
   </si>
   <si>
-    <t>الحي </t>
+    <t>الحي</t>
   </si>
   <si>
     <t>الشارع</t>
@@ -166,9 +174,6 @@
     <t>سبب الوفاة</t>
   </si>
   <si>
-    <t>15/03/2011</t>
-  </si>
-  <si>
     <t>الأم</t>
   </si>
   <si>
@@ -202,7 +207,7 @@
     <t>مدينة حلب</t>
   </si>
   <si>
-    <t>الحي </t>
+    <t>الحي</t>
   </si>
   <si>
     <t>الشارع</t>
@@ -227,41 +232,56 @@
   </si>
   <si>
     <t>ملاحظات</t>
+  </si>
+  <si>
+    <t>متوفى</t>
+  </si>
+  <si>
+    <t>15/03/2018</t>
+  </si>
+  <si>
+    <t>الأب متوفي؟</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -281,8 +301,14 @@
         <bgColor rgb="FFD8D8D8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF79646"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -299,6 +325,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -311,6 +338,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -325,6 +353,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -337,6 +366,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -349,6 +379,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -361,6 +392,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -373,6 +405,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -383,6 +416,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -395,6 +429,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -409,6 +444,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -421,6 +457,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -435,6 +472,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -449,6 +487,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -463,6 +502,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -475,6 +515,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -487,6 +528,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -501,6 +543,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -515,6 +558,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -527,6 +571,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -539,6 +584,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -551,454 +597,882 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="2" applyFont="1" fontId="1" applyFill="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="3" applyFont="1" fontId="2" applyFill="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="4" applyFont="1" fontId="2">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="5" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="6" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="6" applyFont="1" fontId="1" applyFill="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="7" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="8" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="9" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="10" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="11" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="7" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="2" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="12" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="13" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="14" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="12" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="13" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="13" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="14" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="15" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="16" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="16" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="10" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="10" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="17" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="17" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="18" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="19" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="20" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="21" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="19" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="21" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="20" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="21" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="1" borderId="19" applyFont="1" fontId="3" applyNumberFormat="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="19" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="16" applyFont="1" fontId="3">
+  <cellXfs count="44">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM4"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="11.29"/>
-    <col min="2" customWidth="1" max="2" width="15.86"/>
-    <col min="3" customWidth="1" max="3" width="12.43"/>
-    <col min="4" customWidth="1" max="7" width="8.71"/>
-    <col min="8" customWidth="1" max="8" width="14.57"/>
-    <col min="9" customWidth="1" max="9" width="14.29"/>
-    <col min="10" customWidth="1" max="10" width="11.43"/>
-    <col min="11" customWidth="1" max="11" width="10.57"/>
-    <col min="12" customWidth="1" max="15" width="8.71"/>
-    <col min="16" customWidth="1" max="16" width="13.14"/>
-    <col min="17" customWidth="1" max="17" width="8.71"/>
-    <col min="18" customWidth="1" max="18" width="15.0"/>
-    <col min="19" customWidth="1" max="28" width="8.71"/>
-    <col min="29" customWidth="1" max="30" width="13.14"/>
-    <col min="31" customWidth="1" max="31" width="8.71"/>
-    <col min="32" customWidth="1" max="32" width="15.86"/>
-    <col min="33" customWidth="1" max="34" width="9.14"/>
-    <col min="35" customWidth="1" max="37" width="12.0"/>
-    <col min="38" customWidth="1" max="38" width="30.14"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.5" customWidth="1"/>
+    <col min="12" max="12" width="10.5" customWidth="1"/>
+    <col min="13" max="16" width="8.6640625" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" customWidth="1"/>
+    <col min="18" max="18" width="8.6640625" customWidth="1"/>
+    <col min="19" max="19" width="15" customWidth="1"/>
+    <col min="20" max="29" width="8.6640625" customWidth="1"/>
+    <col min="30" max="31" width="13.1640625" customWidth="1"/>
+    <col min="32" max="32" width="8.6640625" customWidth="1"/>
+    <col min="33" max="33" width="15.83203125" customWidth="1"/>
+    <col min="34" max="35" width="9.1640625" customWidth="1"/>
+    <col min="36" max="38" width="12" customWidth="1"/>
+    <col min="39" max="39" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" r="1" ht="25.5">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:39" ht="25.5" customHeight="1">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="2" r="B1">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="3" r="C1">
+      <c r="C1" s="34" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="4" r="K1">
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="35" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="3" r="S1">
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="34" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="5" r="AE1">
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="33" t="s">
         <v>5</v>
       </c>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="27"/>
+      <c r="AI1" s="27"/>
+      <c r="AJ1" s="27"/>
+      <c r="AK1" s="27"/>
+      <c r="AL1" s="27"/>
+      <c r="AM1" s="27"/>
     </row>
-    <row customHeight="1" r="2" ht="29.25">
-      <c t="s" s="6" r="C2">
+    <row r="2" spans="1:39" ht="29.25" customHeight="1">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="7" r="D2">
+      <c r="D2" s="37" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="8" r="E2">
+      <c r="E2" s="38" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="8" r="F2">
+      <c r="F2" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="38" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="8" r="G2">
+      <c r="H2" s="38" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="7" r="H2">
+      <c r="I2" s="37" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="7" r="I2">
+      <c r="J2" s="37" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="9" r="J2">
+      <c r="K2" s="41" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="6" r="K2">
+      <c r="L2" s="28" t="s">
         <v>14</v>
       </c>
-      <c t="s" s="7" r="L2">
+      <c r="M2" s="37" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="8" r="M2">
+      <c r="N2" s="38" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="8" r="N2">
+      <c r="O2" s="38" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="10" r="O2">
+      <c r="P2" s="39" t="s">
         <v>18</v>
       </c>
-      <c t="s" s="11" r="P2">
+      <c r="Q2" s="36" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="12" r="S2">
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="31" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="13" r="X2">
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="32" t="s">
         <v>21</v>
       </c>
-      <c t="s" s="6" r="AC2">
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="28" t="s">
         <v>22</v>
       </c>
-      <c t="s" s="14" r="AD2">
+      <c r="AE2" s="29" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="6" r="AE2">
+      <c r="AF2" s="28" t="s">
         <v>24</v>
       </c>
-      <c t="s" s="14" r="AF2">
+      <c r="AG2" s="29" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="6" r="AG2">
+      <c r="AH2" s="28" t="s">
         <v>26</v>
       </c>
-      <c t="s" s="14" r="AH2">
+      <c r="AI2" s="29" t="s">
         <v>27</v>
       </c>
-      <c t="s" s="2" r="AI2">
+      <c r="AJ2" s="30" t="s">
         <v>28</v>
       </c>
-      <c t="s" s="15" r="AJ2">
+      <c r="AK2" s="26" t="s">
         <v>29</v>
       </c>
-      <c t="s" s="15" r="AK2">
+      <c r="AL2" s="26" t="s">
         <v>30</v>
       </c>
-      <c t="s" s="15" r="AL2">
+      <c r="AM2" s="26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row customHeight="1" r="3" ht="29.25">
-      <c t="s" s="16" r="P3">
+    <row r="3" spans="1:39" ht="29.25" customHeight="1">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="1" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="17" r="Q3">
+      <c r="R3" s="2" t="s">
         <v>33</v>
       </c>
-      <c t="s" s="18" r="R3">
+      <c r="S3" s="3" t="s">
         <v>34</v>
       </c>
-      <c t="s" s="19" r="S3">
+      <c r="T3" s="4" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="20" r="T3">
+      <c r="U3" s="5" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="20" r="U3">
+      <c r="V3" s="5" t="s">
         <v>37</v>
       </c>
-      <c t="s" s="21" r="V3">
+      <c r="W3" s="6" t="s">
         <v>38</v>
       </c>
-      <c t="s" s="22" r="W3">
+      <c r="X3" s="7" t="s">
         <v>39</v>
       </c>
-      <c t="s" s="23" r="X3">
+      <c r="Y3" s="8" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="20" r="Y3">
+      <c r="Z3" s="5" t="s">
         <v>41</v>
       </c>
-      <c t="s" s="20" r="Z3">
+      <c r="AA3" s="5" t="s">
         <v>42</v>
       </c>
-      <c t="s" s="21" r="AA3">
+      <c r="AB3" s="6" t="s">
         <v>43</v>
       </c>
-      <c t="s" s="22" r="AB3">
+      <c r="AC3" s="7" t="s">
         <v>44</v>
       </c>
+      <c r="AD3" s="27"/>
+      <c r="AE3" s="27"/>
+      <c r="AF3" s="27"/>
+      <c r="AG3" s="27"/>
+      <c r="AH3" s="27"/>
+      <c r="AI3" s="27"/>
+      <c r="AJ3" s="27"/>
+      <c r="AK3" s="27"/>
+      <c r="AL3" s="27"/>
+      <c r="AM3" s="27"/>
     </row>
-    <row customHeight="1" r="4" ht="23.25">
-      <c s="24" r="A4">
-        <v>1.0</v>
-      </c>
-      <c t="s" s="25" r="B4">
+    <row r="4" spans="1:39" ht="23.25" customHeight="1">
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>45</v>
       </c>
-      <c t="s" s="26" r="C4">
+      <c r="C4" s="11" t="s">
         <v>46</v>
       </c>
-      <c t="s" s="27" r="D4">
+      <c r="D4" s="12" t="s">
         <v>47</v>
       </c>
-      <c t="s" s="28" r="E4">
+      <c r="E4" s="13" t="s">
         <v>48</v>
       </c>
-      <c t="s" s="28" r="F4">
+      <c r="F4" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>49</v>
       </c>
-      <c t="s" s="28" r="G4">
+      <c r="H4" s="13" t="s">
         <v>50</v>
       </c>
-      <c t="s" s="29" r="H4">
+      <c r="I4" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>51</v>
       </c>
-      <c t="s" s="28" r="I4">
+      <c r="K4" s="15" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="30" r="J4">
+      <c r="L4" s="12" t="s">
         <v>53</v>
       </c>
-      <c t="s" s="27" r="K4">
+      <c r="M4" s="13" t="s">
         <v>54</v>
       </c>
-      <c t="s" s="28" r="L4">
+      <c r="N4" s="13" t="s">
         <v>55</v>
       </c>
-      <c t="s" s="28" r="M4">
+      <c r="O4" s="13" t="s">
         <v>56</v>
       </c>
-      <c t="s" s="28" r="N4">
+      <c r="P4" s="12" t="s">
         <v>57</v>
       </c>
-      <c t="s" s="27" r="O4">
+      <c r="Q4" s="16" t="s">
         <v>58</v>
       </c>
-      <c t="s" s="31" r="P4">
+      <c r="R4" s="17" t="s">
         <v>59</v>
       </c>
-      <c t="s" s="32" r="Q4">
+      <c r="S4" s="18">
+        <v>448273</v>
+      </c>
+      <c r="T4" s="19" t="s">
         <v>60</v>
       </c>
-      <c s="33" r="R4">
-        <v>448273.0</v>
-      </c>
-      <c t="s" s="34" r="S4">
+      <c r="U4" s="17" t="s">
         <v>61</v>
       </c>
-      <c t="s" s="32" r="T4">
+      <c r="V4" s="17" t="s">
         <v>62</v>
       </c>
-      <c t="s" s="32" r="U4">
+      <c r="W4" s="17" t="s">
         <v>63</v>
       </c>
-      <c t="s" s="32" r="V4">
+      <c r="X4" s="20"/>
+      <c r="Y4" s="19" t="s">
         <v>64</v>
       </c>
-      <c s="35" r="W4"/>
-      <c t="s" s="34" r="X4">
+      <c r="Z4" s="17" t="s">
         <v>65</v>
       </c>
-      <c t="s" s="32" r="Y4">
+      <c r="AA4" s="17" t="s">
         <v>66</v>
       </c>
-      <c t="s" s="32" r="Z4">
+      <c r="AB4" s="21"/>
+      <c r="AC4" s="22" t="s">
         <v>67</v>
       </c>
-      <c s="36" r="AA4"/>
-      <c t="s" s="37" r="AB4">
+      <c r="AD4" s="23">
+        <v>998716</v>
+      </c>
+      <c r="AE4" s="22" t="s">
         <v>68</v>
       </c>
-      <c s="38" r="AC4">
-        <v>998716.0</v>
-      </c>
-      <c t="s" s="37" r="AD4">
+      <c r="AF4" s="24" t="s">
         <v>69</v>
       </c>
-      <c t="s" s="39" r="AE4">
+      <c r="AG4" s="20"/>
+      <c r="AH4" s="24">
+        <v>7</v>
+      </c>
+      <c r="AI4" s="18">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="9"/>
+      <c r="AK4" s="9"/>
+      <c r="AL4" s="9"/>
+      <c r="AM4" s="25" t="s">
         <v>70</v>
-      </c>
-      <c s="35" r="AF4"/>
-      <c s="39" r="AG4">
-        <v>7.0</v>
-      </c>
-      <c s="33" r="AH4">
-        <v>0.0</v>
-      </c>
-      <c s="24" r="AI4"/>
-      <c s="24" r="AJ4"/>
-      <c s="24" r="AK4"/>
-      <c t="s" s="40" r="AL4">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="AL2:AL3"/>
-    <mergeCell ref="AK2:AK3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AC2:AC3"/>
+  <mergeCells count="33">
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="AF1:AM1"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="L1:S1"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="T1:AE1"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
     <mergeCell ref="AD2:AD3"/>
     <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="T2:X2"/>
+    <mergeCell ref="Y2:AC2"/>
+    <mergeCell ref="AM2:AM3"/>
+    <mergeCell ref="AL2:AL3"/>
     <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="S2:W2"/>
-    <mergeCell ref="X2:AB2"/>
-    <mergeCell ref="AE1:AL1"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="K1:R1"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S1:AD1"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AK2:AK3"/>
+    <mergeCell ref="AJ2:AJ3"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added validations for father_alive, father_is_martyr and father_date_of_death values
</commit_message>
<xml_diff>
--- a/spec/fixtures/one_orphan_xlsx.xlsx
+++ b/spec/fixtures/one_orphan_xlsx.xlsx
@@ -237,10 +237,10 @@
     <t>متوفى</t>
   </si>
   <si>
-    <t>15/03/2018</t>
-  </si>
-  <si>
     <t>الأب متوفي؟</t>
+  </si>
+  <si>
+    <t>15/03/2011</t>
   </si>
 </sst>
 </file>
@@ -698,56 +698,56 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1084,7 +1084,7 @@
   <dimension ref="A1:AM4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1111,10 +1111,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="25.5" customHeight="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="34" t="s">
@@ -1166,22 +1166,22 @@
     <row r="2" spans="1:39" ht="29.25" customHeight="1">
       <c r="A2" s="27"/>
       <c r="B2" s="27"/>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="38" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="38" t="s">
+      <c r="F2" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="H2" s="29" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="37" t="s">
@@ -1190,19 +1190,19 @@
       <c r="J2" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="41" t="s">
+      <c r="K2" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="L2" s="38" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="38" t="s">
+      <c r="N2" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="38" t="s">
+      <c r="O2" s="29" t="s">
         <v>17</v>
       </c>
       <c r="P2" s="39" t="s">
@@ -1213,48 +1213,48 @@
       </c>
       <c r="R2" s="27"/>
       <c r="S2" s="27"/>
-      <c r="T2" s="31" t="s">
+      <c r="T2" s="41" t="s">
         <v>20</v>
       </c>
       <c r="U2" s="27"/>
       <c r="V2" s="27"/>
       <c r="W2" s="27"/>
       <c r="X2" s="27"/>
-      <c r="Y2" s="32" t="s">
+      <c r="Y2" s="42" t="s">
         <v>21</v>
       </c>
       <c r="Z2" s="27"/>
       <c r="AA2" s="27"/>
       <c r="AB2" s="27"/>
       <c r="AC2" s="27"/>
-      <c r="AD2" s="28" t="s">
+      <c r="AD2" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="AE2" s="29" t="s">
+      <c r="AE2" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AF2" s="28" t="s">
+      <c r="AF2" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="AG2" s="29" t="s">
+      <c r="AG2" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="AH2" s="28" t="s">
+      <c r="AH2" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="AI2" s="29" t="s">
+      <c r="AI2" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="AJ2" s="30" t="s">
+      <c r="AJ2" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="AK2" s="26" t="s">
+      <c r="AK2" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AL2" s="26" t="s">
+      <c r="AL2" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="AM2" s="26" t="s">
+      <c r="AM2" s="43" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1264,7 +1264,7 @@
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
-      <c r="F3" s="43"/>
+      <c r="F3" s="32"/>
       <c r="G3" s="27"/>
       <c r="H3" s="27"/>
       <c r="I3" s="27"/>
@@ -1351,7 +1351,7 @@
         <v>50</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J4" s="13" t="s">
         <v>51</v>
@@ -1434,11 +1434,18 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="AM2:AM3"/>
+    <mergeCell ref="AL2:AL3"/>
+    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AK2:AK3"/>
+    <mergeCell ref="AJ2:AJ3"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="T2:X2"/>
+    <mergeCell ref="Y2:AC2"/>
     <mergeCell ref="AF1:AM1"/>
     <mergeCell ref="C1:K1"/>
     <mergeCell ref="L1:S1"/>
@@ -1455,18 +1462,11 @@
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="P2:P3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="T2:X2"/>
-    <mergeCell ref="Y2:AC2"/>
-    <mergeCell ref="AM2:AM3"/>
-    <mergeCell ref="AL2:AL3"/>
-    <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AK2:AK3"/>
-    <mergeCell ref="AJ2:AJ3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
merging first refactor with @motasem-salem father_alive story
</commit_message>
<xml_diff>
--- a/spec/fixtures/one_orphan_xlsx.xlsx
+++ b/spec/fixtures/one_orphan_xlsx.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <workbookPr autoCompressPictures="0"/>
+  <bookViews>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" tabRatio="500"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>الرقم المسلسل</t>
   </si>
@@ -109,7 +117,7 @@
     <t>ملاحظات</t>
   </si>
   <si>
-    <t>الاسم </t>
+    <t>الاسم</t>
   </si>
   <si>
     <t>صلة القرابة</t>
@@ -124,7 +132,7 @@
     <t>المدينة</t>
   </si>
   <si>
-    <t>الحي </t>
+    <t>الحي</t>
   </si>
   <si>
     <t>الشارع</t>
@@ -139,7 +147,7 @@
     <t>المدينة</t>
   </si>
   <si>
-    <t>الحي </t>
+    <t>الحي</t>
   </si>
   <si>
     <t>الشارع</t>
@@ -166,102 +174,114 @@
     <t>سبب الوفاة</t>
   </si>
   <si>
+    <t>الأم</t>
+  </si>
+  <si>
+    <t>موجودة</t>
+  </si>
+  <si>
+    <t>15/03/2009</t>
+  </si>
+  <si>
+    <t>ذكر</t>
+  </si>
+  <si>
+    <t>معافى</t>
+  </si>
+  <si>
+    <t>الصف الرابع</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>الوصي</t>
+  </si>
+  <si>
+    <t>عم</t>
+  </si>
+  <si>
+    <t>حلب</t>
+  </si>
+  <si>
+    <t>مدينة حلب</t>
+  </si>
+  <si>
+    <t>الحي</t>
+  </si>
+  <si>
+    <t>الشارع</t>
+  </si>
+  <si>
+    <t>حمص</t>
+  </si>
+  <si>
+    <t>مدينة حمص</t>
+  </si>
+  <si>
+    <t>حي</t>
+  </si>
+  <si>
+    <t>تفصيل</t>
+  </si>
+  <si>
+    <t>رقم آخر</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>ملاحظات</t>
+  </si>
+  <si>
+    <t>متوفى</t>
+  </si>
+  <si>
+    <t>الأب متوفي؟</t>
+  </si>
+  <si>
     <t>15/03/2011</t>
-  </si>
-  <si>
-    <t>الأم</t>
-  </si>
-  <si>
-    <t>موجودة</t>
-  </si>
-  <si>
-    <t>15/03/2009</t>
-  </si>
-  <si>
-    <t>ذكر</t>
-  </si>
-  <si>
-    <t>معافى</t>
-  </si>
-  <si>
-    <t>الصف الرابع</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>الوصي</t>
-  </si>
-  <si>
-    <t>عم</t>
-  </si>
-  <si>
-    <t>حلب</t>
-  </si>
-  <si>
-    <t>مدينة حلب</t>
-  </si>
-  <si>
-    <t>الحي </t>
-  </si>
-  <si>
-    <t>الشارع</t>
-  </si>
-  <si>
-    <t>حمص</t>
-  </si>
-  <si>
-    <t>مدينة حمص</t>
-  </si>
-  <si>
-    <t>حي</t>
-  </si>
-  <si>
-    <t>تفصيل</t>
-  </si>
-  <si>
-    <t>رقم آخر</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>ملاحظات</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -281,8 +301,14 @@
         <bgColor rgb="FFD8D8D8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF79646"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -299,6 +325,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -311,6 +338,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -325,6 +353,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -337,6 +366,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -349,6 +379,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -361,6 +392,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -373,6 +405,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -383,6 +416,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -395,6 +429,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -409,6 +444,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -421,6 +457,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -435,6 +472,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -449,6 +487,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -463,6 +502,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -475,6 +515,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -487,6 +528,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -501,6 +543,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -515,6 +558,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -527,6 +571,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -539,6 +584,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -551,454 +597,882 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="2" applyFont="1" fontId="1" applyFill="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="3" applyFont="1" fontId="2" applyFill="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="4" applyFont="1" fontId="2">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="5" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="6" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="6" applyFont="1" fontId="1" applyFill="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="7" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="8" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="9" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="10" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="11" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="7" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="2" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="12" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="13" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="14" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="12" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="13" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="13" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="14" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="15" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="16" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="16" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="10" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="10" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="17" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="17" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="18" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="19" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="20" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="21" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="19" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="21" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="20" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="21" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="1" borderId="19" applyFont="1" fontId="3" applyNumberFormat="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="19" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="16" applyFont="1" fontId="3">
+  <cellXfs count="44">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM4"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="11.29"/>
-    <col min="2" customWidth="1" max="2" width="15.86"/>
-    <col min="3" customWidth="1" max="3" width="12.43"/>
-    <col min="4" customWidth="1" max="7" width="8.71"/>
-    <col min="8" customWidth="1" max="8" width="14.57"/>
-    <col min="9" customWidth="1" max="9" width="14.29"/>
-    <col min="10" customWidth="1" max="10" width="11.43"/>
-    <col min="11" customWidth="1" max="11" width="10.57"/>
-    <col min="12" customWidth="1" max="15" width="8.71"/>
-    <col min="16" customWidth="1" max="16" width="13.14"/>
-    <col min="17" customWidth="1" max="17" width="8.71"/>
-    <col min="18" customWidth="1" max="18" width="15.0"/>
-    <col min="19" customWidth="1" max="28" width="8.71"/>
-    <col min="29" customWidth="1" max="30" width="13.14"/>
-    <col min="31" customWidth="1" max="31" width="8.71"/>
-    <col min="32" customWidth="1" max="32" width="15.86"/>
-    <col min="33" customWidth="1" max="34" width="9.14"/>
-    <col min="35" customWidth="1" max="37" width="12.0"/>
-    <col min="38" customWidth="1" max="38" width="30.14"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.5" customWidth="1"/>
+    <col min="12" max="12" width="10.5" customWidth="1"/>
+    <col min="13" max="16" width="8.6640625" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" customWidth="1"/>
+    <col min="18" max="18" width="8.6640625" customWidth="1"/>
+    <col min="19" max="19" width="15" customWidth="1"/>
+    <col min="20" max="29" width="8.6640625" customWidth="1"/>
+    <col min="30" max="31" width="13.1640625" customWidth="1"/>
+    <col min="32" max="32" width="8.6640625" customWidth="1"/>
+    <col min="33" max="33" width="15.83203125" customWidth="1"/>
+    <col min="34" max="35" width="9.1640625" customWidth="1"/>
+    <col min="36" max="38" width="12" customWidth="1"/>
+    <col min="39" max="39" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" r="1" ht="25.5">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:39" ht="25.5" customHeight="1">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="2" r="B1">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="3" r="C1">
+      <c r="C1" s="34" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="4" r="K1">
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="35" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="3" r="S1">
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="34" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="5" r="AE1">
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="33" t="s">
         <v>5</v>
       </c>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="27"/>
+      <c r="AI1" s="27"/>
+      <c r="AJ1" s="27"/>
+      <c r="AK1" s="27"/>
+      <c r="AL1" s="27"/>
+      <c r="AM1" s="27"/>
     </row>
-    <row customHeight="1" r="2" ht="29.25">
-      <c t="s" s="6" r="C2">
+    <row r="2" spans="1:39" ht="29.25" customHeight="1">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="38" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="7" r="D2">
+      <c r="D2" s="37" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="8" r="E2">
+      <c r="E2" s="29" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="8" r="F2">
+      <c r="F2" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="29" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="8" r="G2">
+      <c r="H2" s="29" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="7" r="H2">
+      <c r="I2" s="37" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="7" r="I2">
+      <c r="J2" s="37" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="9" r="J2">
+      <c r="K2" s="30" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="6" r="K2">
+      <c r="L2" s="38" t="s">
         <v>14</v>
       </c>
-      <c t="s" s="7" r="L2">
+      <c r="M2" s="37" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="8" r="M2">
+      <c r="N2" s="29" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="8" r="N2">
+      <c r="O2" s="29" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="10" r="O2">
+      <c r="P2" s="39" t="s">
         <v>18</v>
       </c>
-      <c t="s" s="11" r="P2">
+      <c r="Q2" s="36" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="12" r="S2">
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="41" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="13" r="X2">
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="42" t="s">
         <v>21</v>
       </c>
-      <c t="s" s="6" r="AC2">
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="38" t="s">
         <v>22</v>
       </c>
-      <c t="s" s="14" r="AD2">
+      <c r="AE2" s="40" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="6" r="AE2">
+      <c r="AF2" s="38" t="s">
         <v>24</v>
       </c>
-      <c t="s" s="14" r="AF2">
+      <c r="AG2" s="40" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="6" r="AG2">
+      <c r="AH2" s="38" t="s">
         <v>26</v>
       </c>
-      <c t="s" s="14" r="AH2">
+      <c r="AI2" s="40" t="s">
         <v>27</v>
       </c>
-      <c t="s" s="2" r="AI2">
+      <c r="AJ2" s="26" t="s">
         <v>28</v>
       </c>
-      <c t="s" s="15" r="AJ2">
+      <c r="AK2" s="43" t="s">
         <v>29</v>
       </c>
-      <c t="s" s="15" r="AK2">
+      <c r="AL2" s="43" t="s">
         <v>30</v>
       </c>
-      <c t="s" s="15" r="AL2">
+      <c r="AM2" s="43" t="s">
         <v>31</v>
       </c>
     </row>
-    <row customHeight="1" r="3" ht="29.25">
-      <c t="s" s="16" r="P3">
+    <row r="3" spans="1:39" ht="29.25" customHeight="1">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="1" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="17" r="Q3">
+      <c r="R3" s="2" t="s">
         <v>33</v>
       </c>
-      <c t="s" s="18" r="R3">
+      <c r="S3" s="3" t="s">
         <v>34</v>
       </c>
-      <c t="s" s="19" r="S3">
+      <c r="T3" s="4" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="20" r="T3">
+      <c r="U3" s="5" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="20" r="U3">
+      <c r="V3" s="5" t="s">
         <v>37</v>
       </c>
-      <c t="s" s="21" r="V3">
+      <c r="W3" s="6" t="s">
         <v>38</v>
       </c>
-      <c t="s" s="22" r="W3">
+      <c r="X3" s="7" t="s">
         <v>39</v>
       </c>
-      <c t="s" s="23" r="X3">
+      <c r="Y3" s="8" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="20" r="Y3">
+      <c r="Z3" s="5" t="s">
         <v>41</v>
       </c>
-      <c t="s" s="20" r="Z3">
+      <c r="AA3" s="5" t="s">
         <v>42</v>
       </c>
-      <c t="s" s="21" r="AA3">
+      <c r="AB3" s="6" t="s">
         <v>43</v>
       </c>
-      <c t="s" s="22" r="AB3">
+      <c r="AC3" s="7" t="s">
         <v>44</v>
       </c>
+      <c r="AD3" s="27"/>
+      <c r="AE3" s="27"/>
+      <c r="AF3" s="27"/>
+      <c r="AG3" s="27"/>
+      <c r="AH3" s="27"/>
+      <c r="AI3" s="27"/>
+      <c r="AJ3" s="27"/>
+      <c r="AK3" s="27"/>
+      <c r="AL3" s="27"/>
+      <c r="AM3" s="27"/>
     </row>
-    <row customHeight="1" r="4" ht="23.25">
-      <c s="24" r="A4">
-        <v>1.0</v>
-      </c>
-      <c t="s" s="25" r="B4">
+    <row r="4" spans="1:39" ht="23.25" customHeight="1">
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>45</v>
       </c>
-      <c t="s" s="26" r="C4">
+      <c r="C4" s="11" t="s">
         <v>46</v>
       </c>
-      <c t="s" s="27" r="D4">
+      <c r="D4" s="12" t="s">
         <v>47</v>
       </c>
-      <c t="s" s="28" r="E4">
+      <c r="E4" s="13" t="s">
         <v>48</v>
       </c>
-      <c t="s" s="28" r="F4">
+      <c r="F4" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>49</v>
       </c>
-      <c t="s" s="28" r="G4">
+      <c r="H4" s="13" t="s">
         <v>50</v>
       </c>
-      <c t="s" s="29" r="H4">
+      <c r="I4" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>51</v>
       </c>
-      <c t="s" s="28" r="I4">
+      <c r="K4" s="15" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="30" r="J4">
+      <c r="L4" s="12" t="s">
         <v>53</v>
       </c>
-      <c t="s" s="27" r="K4">
+      <c r="M4" s="13" t="s">
         <v>54</v>
       </c>
-      <c t="s" s="28" r="L4">
+      <c r="N4" s="13" t="s">
         <v>55</v>
       </c>
-      <c t="s" s="28" r="M4">
+      <c r="O4" s="13" t="s">
         <v>56</v>
       </c>
-      <c t="s" s="28" r="N4">
+      <c r="P4" s="12" t="s">
         <v>57</v>
       </c>
-      <c t="s" s="27" r="O4">
+      <c r="Q4" s="16" t="s">
         <v>58</v>
       </c>
-      <c t="s" s="31" r="P4">
+      <c r="R4" s="17" t="s">
         <v>59</v>
       </c>
-      <c t="s" s="32" r="Q4">
+      <c r="S4" s="18">
+        <v>448273</v>
+      </c>
+      <c r="T4" s="19" t="s">
         <v>60</v>
       </c>
-      <c s="33" r="R4">
-        <v>448273.0</v>
-      </c>
-      <c t="s" s="34" r="S4">
+      <c r="U4" s="17" t="s">
         <v>61</v>
       </c>
-      <c t="s" s="32" r="T4">
+      <c r="V4" s="17" t="s">
         <v>62</v>
       </c>
-      <c t="s" s="32" r="U4">
+      <c r="W4" s="17" t="s">
         <v>63</v>
       </c>
-      <c t="s" s="32" r="V4">
+      <c r="X4" s="20"/>
+      <c r="Y4" s="19" t="s">
         <v>64</v>
       </c>
-      <c s="35" r="W4"/>
-      <c t="s" s="34" r="X4">
+      <c r="Z4" s="17" t="s">
         <v>65</v>
       </c>
-      <c t="s" s="32" r="Y4">
+      <c r="AA4" s="17" t="s">
         <v>66</v>
       </c>
-      <c t="s" s="32" r="Z4">
+      <c r="AB4" s="21"/>
+      <c r="AC4" s="22" t="s">
         <v>67</v>
       </c>
-      <c s="36" r="AA4"/>
-      <c t="s" s="37" r="AB4">
+      <c r="AD4" s="23">
+        <v>998716</v>
+      </c>
+      <c r="AE4" s="22" t="s">
         <v>68</v>
       </c>
-      <c s="38" r="AC4">
-        <v>998716.0</v>
-      </c>
-      <c t="s" s="37" r="AD4">
+      <c r="AF4" s="24" t="s">
         <v>69</v>
       </c>
-      <c t="s" s="39" r="AE4">
+      <c r="AG4" s="20"/>
+      <c r="AH4" s="24">
+        <v>7</v>
+      </c>
+      <c r="AI4" s="18">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="9"/>
+      <c r="AK4" s="9"/>
+      <c r="AL4" s="9"/>
+      <c r="AM4" s="25" t="s">
         <v>70</v>
-      </c>
-      <c s="35" r="AF4"/>
-      <c s="39" r="AG4">
-        <v>7.0</v>
-      </c>
-      <c s="33" r="AH4">
-        <v>0.0</v>
-      </c>
-      <c s="24" r="AI4"/>
-      <c s="24" r="AJ4"/>
-      <c s="24" r="AK4"/>
-      <c t="s" s="40" r="AL4">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="33">
+    <mergeCell ref="AM2:AM3"/>
     <mergeCell ref="AL2:AL3"/>
+    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="AG2:AG3"/>
     <mergeCell ref="AK2:AK3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AF2:AF3"/>
     <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AC2:AC3"/>
     <mergeCell ref="AD2:AD3"/>
     <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="S2:W2"/>
-    <mergeCell ref="X2:AB2"/>
-    <mergeCell ref="AE1:AL1"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="K1:R1"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S1:AD1"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="T2:X2"/>
+    <mergeCell ref="Y2:AC2"/>
+    <mergeCell ref="AF1:AM1"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="L1:S1"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="T1:AE1"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="I2:I3"/>
     <mergeCell ref="H2:H3"/>
+    <mergeCell ref="C2:C3"/>
     <mergeCell ref="G2:G3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="J2:J3"/>
     <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="A1:A3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
merging first refactor with @mots father_alive story
</commit_message>
<xml_diff>
--- a/spec/fixtures/one_orphan_xlsx.xlsx
+++ b/spec/fixtures/one_orphan_xlsx.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <workbookPr autoCompressPictures="0"/>
+  <bookViews>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" tabRatio="500"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>الرقم المسلسل</t>
   </si>
@@ -109,7 +117,7 @@
     <t>ملاحظات</t>
   </si>
   <si>
-    <t>الاسم </t>
+    <t>الاسم</t>
   </si>
   <si>
     <t>صلة القرابة</t>
@@ -124,7 +132,7 @@
     <t>المدينة</t>
   </si>
   <si>
-    <t>الحي </t>
+    <t>الحي</t>
   </si>
   <si>
     <t>الشارع</t>
@@ -139,7 +147,7 @@
     <t>المدينة</t>
   </si>
   <si>
-    <t>الحي </t>
+    <t>الحي</t>
   </si>
   <si>
     <t>الشارع</t>
@@ -166,102 +174,114 @@
     <t>سبب الوفاة</t>
   </si>
   <si>
+    <t>الأم</t>
+  </si>
+  <si>
+    <t>موجودة</t>
+  </si>
+  <si>
+    <t>15/03/2009</t>
+  </si>
+  <si>
+    <t>ذكر</t>
+  </si>
+  <si>
+    <t>معافى</t>
+  </si>
+  <si>
+    <t>الصف الرابع</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>الوصي</t>
+  </si>
+  <si>
+    <t>عم</t>
+  </si>
+  <si>
+    <t>حلب</t>
+  </si>
+  <si>
+    <t>مدينة حلب</t>
+  </si>
+  <si>
+    <t>الحي</t>
+  </si>
+  <si>
+    <t>الشارع</t>
+  </si>
+  <si>
+    <t>حمص</t>
+  </si>
+  <si>
+    <t>مدينة حمص</t>
+  </si>
+  <si>
+    <t>حي</t>
+  </si>
+  <si>
+    <t>تفصيل</t>
+  </si>
+  <si>
+    <t>رقم آخر</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>ملاحظات</t>
+  </si>
+  <si>
+    <t>متوفى</t>
+  </si>
+  <si>
+    <t>الأب متوفي؟</t>
+  </si>
+  <si>
     <t>15/03/2011</t>
-  </si>
-  <si>
-    <t>الأم</t>
-  </si>
-  <si>
-    <t>موجودة</t>
-  </si>
-  <si>
-    <t>15/03/2009</t>
-  </si>
-  <si>
-    <t>ذكر</t>
-  </si>
-  <si>
-    <t>معافى</t>
-  </si>
-  <si>
-    <t>الصف الرابع</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>الوصي</t>
-  </si>
-  <si>
-    <t>عم</t>
-  </si>
-  <si>
-    <t>حلب</t>
-  </si>
-  <si>
-    <t>مدينة حلب</t>
-  </si>
-  <si>
-    <t>الحي </t>
-  </si>
-  <si>
-    <t>الشارع</t>
-  </si>
-  <si>
-    <t>حمص</t>
-  </si>
-  <si>
-    <t>مدينة حمص</t>
-  </si>
-  <si>
-    <t>حي</t>
-  </si>
-  <si>
-    <t>تفصيل</t>
-  </si>
-  <si>
-    <t>رقم آخر</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>ملاحظات</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -281,8 +301,14 @@
         <bgColor rgb="FFD8D8D8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF79646"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -299,6 +325,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -311,6 +338,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -325,6 +353,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -337,6 +366,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -349,6 +379,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -361,6 +392,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -373,6 +405,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -383,6 +416,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -395,6 +429,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -409,6 +444,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -421,6 +457,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -435,6 +472,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -449,6 +487,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -463,6 +502,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -475,6 +515,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -487,6 +528,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -501,6 +543,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -515,6 +558,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -527,6 +571,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -539,6 +584,7 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="dotted">
@@ -551,454 +597,882 @@
       <bottom style="dotted">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="2" applyFont="1" fontId="1" applyFill="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="3" applyFont="1" fontId="2" applyFill="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="4" applyFont="1" fontId="2">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="5" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="6" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="6" applyFont="1" fontId="1" applyFill="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="7" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="8" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="9" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="10" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="11" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="7" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="2" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="12" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="13" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="14" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="12" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="13" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="13" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="14" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="15" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="16" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="16" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="10" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="10" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="17" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="17" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="18" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="19" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="20" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="21" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="19" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="21" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="20" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="21" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="1" borderId="19" applyFont="1" fontId="3" applyNumberFormat="1">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="19" applyFont="1" fontId="3">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="16" applyFont="1" fontId="3">
+  <cellXfs count="44">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM4"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="11.29"/>
-    <col min="2" customWidth="1" max="2" width="15.86"/>
-    <col min="3" customWidth="1" max="3" width="12.43"/>
-    <col min="4" customWidth="1" max="7" width="8.71"/>
-    <col min="8" customWidth="1" max="8" width="14.57"/>
-    <col min="9" customWidth="1" max="9" width="14.29"/>
-    <col min="10" customWidth="1" max="10" width="11.43"/>
-    <col min="11" customWidth="1" max="11" width="10.57"/>
-    <col min="12" customWidth="1" max="15" width="8.71"/>
-    <col min="16" customWidth="1" max="16" width="13.14"/>
-    <col min="17" customWidth="1" max="17" width="8.71"/>
-    <col min="18" customWidth="1" max="18" width="15.0"/>
-    <col min="19" customWidth="1" max="28" width="8.71"/>
-    <col min="29" customWidth="1" max="30" width="13.14"/>
-    <col min="31" customWidth="1" max="31" width="8.71"/>
-    <col min="32" customWidth="1" max="32" width="15.86"/>
-    <col min="33" customWidth="1" max="34" width="9.14"/>
-    <col min="35" customWidth="1" max="37" width="12.0"/>
-    <col min="38" customWidth="1" max="38" width="30.14"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.5" customWidth="1"/>
+    <col min="12" max="12" width="10.5" customWidth="1"/>
+    <col min="13" max="16" width="8.6640625" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" customWidth="1"/>
+    <col min="18" max="18" width="8.6640625" customWidth="1"/>
+    <col min="19" max="19" width="15" customWidth="1"/>
+    <col min="20" max="29" width="8.6640625" customWidth="1"/>
+    <col min="30" max="31" width="13.1640625" customWidth="1"/>
+    <col min="32" max="32" width="8.6640625" customWidth="1"/>
+    <col min="33" max="33" width="15.83203125" customWidth="1"/>
+    <col min="34" max="35" width="9.1640625" customWidth="1"/>
+    <col min="36" max="38" width="12" customWidth="1"/>
+    <col min="39" max="39" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" r="1" ht="25.5">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:39" ht="25.5" customHeight="1">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="2" r="B1">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="3" r="C1">
+      <c r="C1" s="34" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="4" r="K1">
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="35" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="3" r="S1">
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="34" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="5" r="AE1">
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="33" t="s">
         <v>5</v>
       </c>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="27"/>
+      <c r="AI1" s="27"/>
+      <c r="AJ1" s="27"/>
+      <c r="AK1" s="27"/>
+      <c r="AL1" s="27"/>
+      <c r="AM1" s="27"/>
     </row>
-    <row customHeight="1" r="2" ht="29.25">
-      <c t="s" s="6" r="C2">
+    <row r="2" spans="1:39" ht="29.25" customHeight="1">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="38" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="7" r="D2">
+      <c r="D2" s="37" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="8" r="E2">
+      <c r="E2" s="29" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="8" r="F2">
+      <c r="F2" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="29" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="8" r="G2">
+      <c r="H2" s="29" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="7" r="H2">
+      <c r="I2" s="37" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="7" r="I2">
+      <c r="J2" s="37" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="9" r="J2">
+      <c r="K2" s="30" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="6" r="K2">
+      <c r="L2" s="38" t="s">
         <v>14</v>
       </c>
-      <c t="s" s="7" r="L2">
+      <c r="M2" s="37" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="8" r="M2">
+      <c r="N2" s="29" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="8" r="N2">
+      <c r="O2" s="29" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="10" r="O2">
+      <c r="P2" s="39" t="s">
         <v>18</v>
       </c>
-      <c t="s" s="11" r="P2">
+      <c r="Q2" s="36" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="12" r="S2">
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="41" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="13" r="X2">
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="42" t="s">
         <v>21</v>
       </c>
-      <c t="s" s="6" r="AC2">
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="38" t="s">
         <v>22</v>
       </c>
-      <c t="s" s="14" r="AD2">
+      <c r="AE2" s="40" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="6" r="AE2">
+      <c r="AF2" s="38" t="s">
         <v>24</v>
       </c>
-      <c t="s" s="14" r="AF2">
+      <c r="AG2" s="40" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="6" r="AG2">
+      <c r="AH2" s="38" t="s">
         <v>26</v>
       </c>
-      <c t="s" s="14" r="AH2">
+      <c r="AI2" s="40" t="s">
         <v>27</v>
       </c>
-      <c t="s" s="2" r="AI2">
+      <c r="AJ2" s="26" t="s">
         <v>28</v>
       </c>
-      <c t="s" s="15" r="AJ2">
+      <c r="AK2" s="43" t="s">
         <v>29</v>
       </c>
-      <c t="s" s="15" r="AK2">
+      <c r="AL2" s="43" t="s">
         <v>30</v>
       </c>
-      <c t="s" s="15" r="AL2">
+      <c r="AM2" s="43" t="s">
         <v>31</v>
       </c>
     </row>
-    <row customHeight="1" r="3" ht="29.25">
-      <c t="s" s="16" r="P3">
+    <row r="3" spans="1:39" ht="29.25" customHeight="1">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="1" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="17" r="Q3">
+      <c r="R3" s="2" t="s">
         <v>33</v>
       </c>
-      <c t="s" s="18" r="R3">
+      <c r="S3" s="3" t="s">
         <v>34</v>
       </c>
-      <c t="s" s="19" r="S3">
+      <c r="T3" s="4" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="20" r="T3">
+      <c r="U3" s="5" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="20" r="U3">
+      <c r="V3" s="5" t="s">
         <v>37</v>
       </c>
-      <c t="s" s="21" r="V3">
+      <c r="W3" s="6" t="s">
         <v>38</v>
       </c>
-      <c t="s" s="22" r="W3">
+      <c r="X3" s="7" t="s">
         <v>39</v>
       </c>
-      <c t="s" s="23" r="X3">
+      <c r="Y3" s="8" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="20" r="Y3">
+      <c r="Z3" s="5" t="s">
         <v>41</v>
       </c>
-      <c t="s" s="20" r="Z3">
+      <c r="AA3" s="5" t="s">
         <v>42</v>
       </c>
-      <c t="s" s="21" r="AA3">
+      <c r="AB3" s="6" t="s">
         <v>43</v>
       </c>
-      <c t="s" s="22" r="AB3">
+      <c r="AC3" s="7" t="s">
         <v>44</v>
       </c>
+      <c r="AD3" s="27"/>
+      <c r="AE3" s="27"/>
+      <c r="AF3" s="27"/>
+      <c r="AG3" s="27"/>
+      <c r="AH3" s="27"/>
+      <c r="AI3" s="27"/>
+      <c r="AJ3" s="27"/>
+      <c r="AK3" s="27"/>
+      <c r="AL3" s="27"/>
+      <c r="AM3" s="27"/>
     </row>
-    <row customHeight="1" r="4" ht="23.25">
-      <c s="24" r="A4">
-        <v>1.0</v>
-      </c>
-      <c t="s" s="25" r="B4">
+    <row r="4" spans="1:39" ht="23.25" customHeight="1">
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>45</v>
       </c>
-      <c t="s" s="26" r="C4">
+      <c r="C4" s="11" t="s">
         <v>46</v>
       </c>
-      <c t="s" s="27" r="D4">
+      <c r="D4" s="12" t="s">
         <v>47</v>
       </c>
-      <c t="s" s="28" r="E4">
+      <c r="E4" s="13" t="s">
         <v>48</v>
       </c>
-      <c t="s" s="28" r="F4">
+      <c r="F4" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>49</v>
       </c>
-      <c t="s" s="28" r="G4">
+      <c r="H4" s="13" t="s">
         <v>50</v>
       </c>
-      <c t="s" s="29" r="H4">
+      <c r="I4" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>51</v>
       </c>
-      <c t="s" s="28" r="I4">
+      <c r="K4" s="15" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="30" r="J4">
+      <c r="L4" s="12" t="s">
         <v>53</v>
       </c>
-      <c t="s" s="27" r="K4">
+      <c r="M4" s="13" t="s">
         <v>54</v>
       </c>
-      <c t="s" s="28" r="L4">
+      <c r="N4" s="13" t="s">
         <v>55</v>
       </c>
-      <c t="s" s="28" r="M4">
+      <c r="O4" s="13" t="s">
         <v>56</v>
       </c>
-      <c t="s" s="28" r="N4">
+      <c r="P4" s="12" t="s">
         <v>57</v>
       </c>
-      <c t="s" s="27" r="O4">
+      <c r="Q4" s="16" t="s">
         <v>58</v>
       </c>
-      <c t="s" s="31" r="P4">
+      <c r="R4" s="17" t="s">
         <v>59</v>
       </c>
-      <c t="s" s="32" r="Q4">
+      <c r="S4" s="18">
+        <v>448273</v>
+      </c>
+      <c r="T4" s="19" t="s">
         <v>60</v>
       </c>
-      <c s="33" r="R4">
-        <v>448273.0</v>
-      </c>
-      <c t="s" s="34" r="S4">
+      <c r="U4" s="17" t="s">
         <v>61</v>
       </c>
-      <c t="s" s="32" r="T4">
+      <c r="V4" s="17" t="s">
         <v>62</v>
       </c>
-      <c t="s" s="32" r="U4">
+      <c r="W4" s="17" t="s">
         <v>63</v>
       </c>
-      <c t="s" s="32" r="V4">
+      <c r="X4" s="20"/>
+      <c r="Y4" s="19" t="s">
         <v>64</v>
       </c>
-      <c s="35" r="W4"/>
-      <c t="s" s="34" r="X4">
+      <c r="Z4" s="17" t="s">
         <v>65</v>
       </c>
-      <c t="s" s="32" r="Y4">
+      <c r="AA4" s="17" t="s">
         <v>66</v>
       </c>
-      <c t="s" s="32" r="Z4">
+      <c r="AB4" s="21"/>
+      <c r="AC4" s="22" t="s">
         <v>67</v>
       </c>
-      <c s="36" r="AA4"/>
-      <c t="s" s="37" r="AB4">
+      <c r="AD4" s="23">
+        <v>998716</v>
+      </c>
+      <c r="AE4" s="22" t="s">
         <v>68</v>
       </c>
-      <c s="38" r="AC4">
-        <v>998716.0</v>
-      </c>
-      <c t="s" s="37" r="AD4">
+      <c r="AF4" s="24" t="s">
         <v>69</v>
       </c>
-      <c t="s" s="39" r="AE4">
+      <c r="AG4" s="20"/>
+      <c r="AH4" s="24">
+        <v>7</v>
+      </c>
+      <c r="AI4" s="18">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="9"/>
+      <c r="AK4" s="9"/>
+      <c r="AL4" s="9"/>
+      <c r="AM4" s="25" t="s">
         <v>70</v>
-      </c>
-      <c s="35" r="AF4"/>
-      <c s="39" r="AG4">
-        <v>7.0</v>
-      </c>
-      <c s="33" r="AH4">
-        <v>0.0</v>
-      </c>
-      <c s="24" r="AI4"/>
-      <c s="24" r="AJ4"/>
-      <c s="24" r="AK4"/>
-      <c t="s" s="40" r="AL4">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="33">
+    <mergeCell ref="AM2:AM3"/>
     <mergeCell ref="AL2:AL3"/>
+    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="AG2:AG3"/>
     <mergeCell ref="AK2:AK3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AF2:AF3"/>
     <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AC2:AC3"/>
     <mergeCell ref="AD2:AD3"/>
     <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="S2:W2"/>
-    <mergeCell ref="X2:AB2"/>
-    <mergeCell ref="AE1:AL1"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="K1:R1"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S1:AD1"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="T2:X2"/>
+    <mergeCell ref="Y2:AC2"/>
+    <mergeCell ref="AF1:AM1"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="L1:S1"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="T1:AE1"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="I2:I3"/>
     <mergeCell ref="H2:H3"/>
+    <mergeCell ref="C2:C3"/>
     <mergeCell ref="G2:G3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="J2:J3"/>
     <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="A1:A3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
OSRA-300 Split Orphan `father_name`: Orphan model
OSRA-302 Update Orphan model to separate `father_name` into `father_given_name`
and `family_name`

 - delete `father_name` column from orphans table
 - add `father_given_name` & `family_name` non-null string columns
 - implement temporary `Orphan#father_name` & `#father_name=` to preserve API
 - update one_orphan_xls(x).xls(x) fixtures with 2-word `father_name`
 - test suite green
</commit_message>
<xml_diff>
--- a/spec/fixtures/one_orphan_xlsx.xlsx
+++ b/spec/fixtures/one_orphan_xlsx.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" tabRatio="500"/>
@@ -159,9 +159,6 @@
     <t>الطفل</t>
   </si>
   <si>
-    <t>الأب</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -241,6 +238,9 @@
   </si>
   <si>
     <t>15/03/2011</t>
+  </si>
+  <si>
+    <t>John Smith</t>
   </si>
 </sst>
 </file>
@@ -698,16 +698,49 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -715,39 +748,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1084,7 +1084,7 @@
   <dimension ref="A1:AM4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1111,10 +1111,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="25.5" customHeight="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="34" t="s">
@@ -1166,22 +1166,22 @@
     <row r="2" spans="1:39" ht="29.25" customHeight="1">
       <c r="A2" s="27"/>
       <c r="B2" s="27"/>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="28" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="29" t="s">
+      <c r="F2" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="38" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="37" t="s">
@@ -1190,19 +1190,19 @@
       <c r="J2" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="L2" s="28" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="N2" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="O2" s="38" t="s">
         <v>17</v>
       </c>
       <c r="P2" s="39" t="s">
@@ -1213,48 +1213,48 @@
       </c>
       <c r="R2" s="27"/>
       <c r="S2" s="27"/>
-      <c r="T2" s="41" t="s">
+      <c r="T2" s="31" t="s">
         <v>20</v>
       </c>
       <c r="U2" s="27"/>
       <c r="V2" s="27"/>
       <c r="W2" s="27"/>
       <c r="X2" s="27"/>
-      <c r="Y2" s="42" t="s">
+      <c r="Y2" s="32" t="s">
         <v>21</v>
       </c>
       <c r="Z2" s="27"/>
       <c r="AA2" s="27"/>
       <c r="AB2" s="27"/>
       <c r="AC2" s="27"/>
-      <c r="AD2" s="38" t="s">
+      <c r="AD2" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="AE2" s="40" t="s">
+      <c r="AE2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="AF2" s="38" t="s">
+      <c r="AF2" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="AG2" s="40" t="s">
+      <c r="AG2" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="AH2" s="38" t="s">
+      <c r="AH2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="AI2" s="40" t="s">
+      <c r="AI2" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="AJ2" s="26" t="s">
+      <c r="AJ2" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="AK2" s="43" t="s">
+      <c r="AK2" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="AL2" s="43" t="s">
+      <c r="AL2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="AM2" s="43" t="s">
+      <c r="AM2" s="26" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1264,7 +1264,7 @@
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
-      <c r="F3" s="32"/>
+      <c r="F3" s="43"/>
       <c r="G3" s="27"/>
       <c r="H3" s="27"/>
       <c r="I3" s="27"/>
@@ -1333,90 +1333,90 @@
         <v>45</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="E4" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="I4" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="J4" s="13" t="s">
+      <c r="K4" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="L4" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="M4" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="N4" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="N4" s="13" t="s">
+      <c r="O4" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="O4" s="13" t="s">
+      <c r="P4" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="P4" s="12" t="s">
+      <c r="Q4" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="Q4" s="16" t="s">
+      <c r="R4" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="R4" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="S4" s="18">
         <v>448273</v>
       </c>
       <c r="T4" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="U4" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="U4" s="17" t="s">
+      <c r="V4" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="V4" s="17" t="s">
+      <c r="W4" s="17" t="s">
         <v>62</v>
-      </c>
-      <c r="W4" s="17" t="s">
-        <v>63</v>
       </c>
       <c r="X4" s="20"/>
       <c r="Y4" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z4" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="Z4" s="17" t="s">
+      <c r="AA4" s="17" t="s">
         <v>65</v>
-      </c>
-      <c r="AA4" s="17" t="s">
-        <v>66</v>
       </c>
       <c r="AB4" s="21"/>
       <c r="AC4" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD4" s="23">
         <v>998716</v>
       </c>
       <c r="AE4" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF4" s="24" t="s">
         <v>68</v>
-      </c>
-      <c r="AF4" s="24" t="s">
-        <v>69</v>
       </c>
       <c r="AG4" s="20"/>
       <c r="AH4" s="24">
@@ -1429,23 +1429,16 @@
       <c r="AK4" s="9"/>
       <c r="AL4" s="9"/>
       <c r="AM4" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="AM2:AM3"/>
-    <mergeCell ref="AL2:AL3"/>
-    <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AK2:AK3"/>
-    <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="T2:X2"/>
-    <mergeCell ref="Y2:AC2"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AF1:AM1"/>
     <mergeCell ref="C1:K1"/>
     <mergeCell ref="L1:S1"/>
@@ -1462,11 +1455,18 @@
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="P2:P3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="T2:X2"/>
+    <mergeCell ref="Y2:AC2"/>
+    <mergeCell ref="AM2:AM3"/>
+    <mergeCell ref="AL2:AL3"/>
+    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AK2:AK3"/>
+    <mergeCell ref="AJ2:AJ3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>